<commit_message>
Concept-Description of the DB
</commit_message>
<xml_diff>
--- a/DB/Drafts/ConceptDB-Description.xlsx
+++ b/DB/Drafts/ConceptDB-Description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WS-P1-Thrifter\DB\Drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1682E42A-E1D5-424C-877C-97EF77D7E235}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4D52A3-DAA7-4645-B523-20310C930FA5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4860" xr2:uid="{12C391B5-D1D9-48B7-B487-F32DF70611D6}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>User</t>
   </si>
@@ -95,9 +95,6 @@
     <t>jacob.edwards71@example.com</t>
   </si>
   <si>
-    <t>(122)-211-5186</t>
-  </si>
-  <si>
     <t>u_birtdate</t>
   </si>
   <si>
@@ -108,13 +105,58 @@
   </si>
   <si>
     <t>Wird auto. Erzeugt</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>VARCHAR(200)</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor...</t>
+  </si>
+  <si>
+    <t>(+43)676 344 5566</t>
+  </si>
+  <si>
+    <t>optional/+43 gets add auto-&gt;PHP</t>
+  </si>
+  <si>
+    <t>VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>optional/NurDateiname bestehend aus Username</t>
+  </si>
+  <si>
+    <t>JEdwars2.jpg</t>
+  </si>
+  <si>
+    <t>Edwars</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>HashValue-&gt;SHA3-224-&gt;Keccak</t>
+  </si>
+  <si>
+    <t>64f977868a7a63bb65ddcd10c587b50ad21fe885fe667c99acc5d6f1</t>
+  </si>
+  <si>
+    <t>VARCHAR(56)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,13 +164,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,16 +202,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +540,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,8 +548,8 @@
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -486,7 +561,7 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
@@ -498,9 +573,12 @@
       <c r="F3" s="1">
         <v>4</v>
       </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
@@ -514,7 +592,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -528,81 +606,136 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>5</v>
       </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="4">
+        <v>35735</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2909</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="F14" s="2">
+        <v>43403.706307870372</v>
+      </c>
+      <c r="G14" t="s">
         <v>24</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DB Drafts->new table(Assets)+data type change(p_price)
</commit_message>
<xml_diff>
--- a/DB/Drafts/ConceptDB-Description.xlsx
+++ b/DB/Drafts/ConceptDB-Description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WS-P1-Thrifter\DB\Drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C321CFEA-FF89-40A3-903E-558BB30546A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA1149C-E598-4527-AC3F-D1F0A32D7FC1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4860" xr2:uid="{12C391B5-D1D9-48B7-B487-F32DF70611D6}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="98">
   <si>
     <t>User</t>
   </si>
@@ -297,13 +297,40 @@
   </si>
   <si>
     <t>s_value</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>a_id</t>
+  </si>
+  <si>
+    <t>a_p_post</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Attribut</t>
+  </si>
+  <si>
+    <t>Datentyp</t>
+  </si>
+  <si>
+    <t>Eigenschaften</t>
+  </si>
+  <si>
+    <t>Daten</t>
+  </si>
+  <si>
+    <t>weitere Infos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +352,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -340,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -348,12 +383,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,10 +414,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift 3" xfId="2" builtinId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -684,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A02ADC-1241-4391-8C4E-B2A497892678}">
-  <dimension ref="B2:G56"/>
+  <dimension ref="B1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,93 +749,100 @@
     <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F4" s="1">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -793,190 +850,187 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>35</v>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="4">
-        <v>35735</v>
+      <c r="F9" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="1">
-        <v>1150</v>
+      <c r="F10" s="4">
+        <v>35735</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1150</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="2">
         <v>43403.706307870372</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F18" s="1">
         <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="1">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>57</v>
+      <c r="F19" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>58</v>
+      <c r="F20" s="1">
+        <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>43403.706307870372</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -984,7 +1038,7 @@
         <v>52</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -993,7 +1047,7 @@
         <v>21</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -1001,7 +1055,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -1010,7 +1064,7 @@
         <v>21</v>
       </c>
       <c r="F24" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -1018,7 +1072,7 @@
         <v>52</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
@@ -1027,7 +1081,7 @@
         <v>21</v>
       </c>
       <c r="F25" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1035,7 +1089,7 @@
         <v>52</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -1044,7 +1098,7 @@
         <v>21</v>
       </c>
       <c r="F26" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1052,261 +1106,317 @@
         <v>52</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="1">
         <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="1">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D31" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="1">
         <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D34" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F39" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="5" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F43" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="5" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>30</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D46" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F47" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="5" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>65</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F51" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="5" t="s">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>65</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>11</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D54" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F55" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D55" t="s">
-        <v>30</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>88</v>
       </c>
       <c r="D56" t="s">
         <v>30</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
config.php | func -> func.inc.php | method changes | user changes | home change | profil changes | reg.php | style changes (login) | wishlist changes
</commit_message>
<xml_diff>
--- a/DB/Drafts/ConceptDB-Description.xlsx
+++ b/DB/Drafts/ConceptDB-Description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WS-P1-Thrifter\DB\Drafts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - HTL Spengergasse\Dokumente\Websites\WS-P1-Thrifter\DB\Drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBA1991-EBE9-464A-9204-DD8A54B5D7E2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBA1991-EBE9-464A-9204-DD8A54B5D7E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4860" xr2:uid="{12C391B5-D1D9-48B7-B487-F32DF70611D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="4860" xr2:uid="{12C391B5-D1D9-48B7-B487-F32DF70611D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -736,20 +736,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A02ADC-1241-4391-8C4E-B2A497892678}">
   <dimension ref="B1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="7" t="s">
         <v>89</v>
       </c>
@@ -769,13 +769,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -795,7 +795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
@@ -809,7 +809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -823,7 +823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
@@ -840,7 +840,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
@@ -854,7 +854,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
@@ -868,7 +868,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
@@ -882,7 +882,7 @@
         <v>35735</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
@@ -896,7 +896,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
@@ -910,7 +910,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
@@ -924,7 +924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
@@ -938,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
@@ -952,12 +952,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -974,7 +974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
@@ -988,7 +988,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
         <v>43</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>43403.706307870372</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>50</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>50</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>50</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>50</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>50</v>
       </c>
@@ -1135,12 +1135,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>57</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>50</v>
       </c>
@@ -1174,12 +1174,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>11</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C36" s="5" t="s">
         <v>71</v>
       </c>
@@ -1207,12 +1207,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>11</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C40" s="5" t="s">
         <v>65</v>
       </c>
@@ -1240,12 +1240,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>11</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C44" s="5" t="s">
         <v>67</v>
       </c>
@@ -1273,12 +1273,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>11</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C48" s="5" t="s">
         <v>73</v>
       </c>
@@ -1306,12 +1306,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>11</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C52" s="5" t="s">
         <v>76</v>
       </c>
@@ -1339,12 +1339,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>11</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C56" s="5" t="s">
         <v>84</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C57" s="5" t="s">
         <v>85</v>
       </c>
@@ -1383,12 +1383,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>11</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C61" s="5" t="s">
         <v>88</v>
       </c>

</xml_diff>